<commit_message>
new images for products/ adding the cart modal/ refactoring the app css and html
</commit_message>
<xml_diff>
--- a/Estimation.xlsx
+++ b/Estimation.xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4BEB99-50D8-4D1D-8B09-03C2FEADF76C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="5880" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -124,12 +131,15 @@
   </si>
   <si>
     <t>testing and bug fixing</t>
+  </si>
+  <si>
+    <t>cart-modal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,22 +460,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.44140625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +489,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -493,7 +503,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -507,7 +517,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -521,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -538,12 +548,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -554,7 +564,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>7</v>
       </c>
@@ -565,7 +575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -576,7 +586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -593,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -610,7 +620,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>12</v>
       </c>
@@ -621,7 +631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -638,12 +648,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>16</v>
       </c>
@@ -654,7 +664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>17</v>
       </c>
@@ -665,7 +675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>18</v>
       </c>
@@ -676,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
@@ -690,7 +700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -707,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>9</v>
       </c>
@@ -718,7 +728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -730,7 +740,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -739,12 +749,12 @@
         <v>59.8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>27</v>
       </c>
@@ -752,7 +762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>28</v>
       </c>
@@ -760,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>29</v>
       </c>
@@ -768,7 +778,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>30</v>
       </c>
@@ -776,7 +786,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>31</v>
       </c>
@@ -784,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -792,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>33</v>
       </c>
@@ -800,12 +810,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>34</v>
       </c>
       <c r="E32">
         <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the estimation file
</commit_message>
<xml_diff>
--- a/Estimation.xlsx
+++ b/Estimation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4BEB99-50D8-4D1D-8B09-03C2FEADF76C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E465340D-7DAA-4CFE-8F4C-B1764DE3ADC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +815,7 @@
         <v>34</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
         <v>35</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>